<commit_message>
Params de la animacion de ayer
</commit_message>
<xml_diff>
--- a/p2/trayectorias.xlsx
+++ b/p2/trayectorias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\cuarto-2\robotica\practicas\p2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\cuarto-2\robotica\practicas\repo\robotica\p2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1532AC-ECD3-48CA-9084-C24456BB57D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BD5D96-2970-4327-8F9F-EE31466A19A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{85F765FC-204A-43B1-828B-4728C7CC8CB9}"/>
   </bookViews>

</xml_diff>